<commit_message>
Fixed up regexes and divide by zero crash
</commit_message>
<xml_diff>
--- a/Assn1/OutputData/test_blockSizeGreaterThanOne.xlsx
+++ b/Assn1/OutputData/test_blockSizeGreaterThanOne.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Github\TeamRocket\Assn1\OutputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\Documents\GitHub\TeamRocket\Assn1\OutputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16180" windowHeight="9500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,9 +363,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -385,384 +385,384 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>33.599998474121094</v>
+        <v>0.39392000436782837</v>
       </c>
       <c r="B2">
-        <v>28.894315719604492</v>
+        <v>0.37689036130905151</v>
       </c>
       <c r="C2">
-        <v>38.305683135986328</v>
+        <v>0.41094964742660522</v>
       </c>
       <c r="E2">
-        <v>2.8009524345397949</v>
+        <v>2.8668475151062012</v>
       </c>
       <c r="F2">
-        <v>2.2343595027923584</v>
+        <v>2.6732652187347412</v>
       </c>
       <c r="G2">
-        <v>3.3675451278686523</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.0604300498962402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>44.639999389648438</v>
+        <v>0.52351999282836914</v>
       </c>
       <c r="B3">
-        <v>40.016746520996094</v>
+        <v>0.50625449419021606</v>
       </c>
       <c r="C3">
-        <v>49.263252258300781</v>
+        <v>0.54078549146652222</v>
       </c>
       <c r="E3">
-        <v>1.9232540130615234</v>
+        <v>2.0024442672729492</v>
       </c>
       <c r="F3">
-        <v>1.7124043703079224</v>
+        <v>1.9128973484039307</v>
       </c>
       <c r="G3">
-        <v>2.134103536605835</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2.0919909477233887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>50.400001525878906</v>
+        <v>0.60048002004623413</v>
       </c>
       <c r="B4">
-        <v>45.992523193359375</v>
+        <v>0.58450525999069214</v>
       </c>
       <c r="C4">
-        <v>54.807476043701172</v>
+        <v>0.61645478010177612</v>
       </c>
       <c r="E4">
-        <v>1.6728571653366089</v>
+        <v>1.6865731477737427</v>
       </c>
       <c r="F4">
-        <v>1.5083465576171875</v>
+        <v>1.6304736137390137</v>
       </c>
       <c r="G4">
-        <v>1.8373676538467407</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.7426726818084717</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>54.720001220703125</v>
+        <v>0.65087997913360596</v>
       </c>
       <c r="B5">
-        <v>50.790107727050781</v>
+        <v>0.63519388437271118</v>
       </c>
       <c r="C5">
-        <v>58.649890899658203</v>
+        <v>0.66656613349914551</v>
       </c>
       <c r="E5">
-        <v>1.5135713815689087</v>
+        <v>1.5434224605560303</v>
       </c>
       <c r="F5">
-        <v>1.3970086574554443</v>
+        <v>1.4946485757827759</v>
       </c>
       <c r="G5">
-        <v>1.6301342248916626</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.5921964645385742</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>57.919998168945313</v>
+        <v>0.69488000869750977</v>
       </c>
       <c r="B6">
-        <v>54.136249542236328</v>
+        <v>0.67959630489349365</v>
       </c>
       <c r="C6">
-        <v>61.703746795654297</v>
+        <v>0.71016371250152588</v>
       </c>
       <c r="E6">
-        <v>1.4238095283508301</v>
+        <v>1.4430468082427979</v>
       </c>
       <c r="F6">
-        <v>1.3173750638961792</v>
+        <v>1.391973614692688</v>
       </c>
       <c r="G6">
-        <v>1.530243992805481</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.4941198825836182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>60.959999084472656</v>
+        <v>0.72703999280929565</v>
       </c>
       <c r="B7">
-        <v>57.376819610595703</v>
+        <v>0.71297943592071533</v>
       </c>
       <c r="C7">
-        <v>64.543182373046875</v>
+        <v>0.74110054969787598</v>
       </c>
       <c r="E7">
-        <v>1.3459523916244507</v>
+        <v>1.361954927444458</v>
       </c>
       <c r="F7">
-        <v>1.2541036605834961</v>
+        <v>1.3231201171875</v>
       </c>
       <c r="G7">
-        <v>1.4378011226654053</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.400789737701416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>62.560001373291016</v>
+        <v>0.74720001220703125</v>
       </c>
       <c r="B8">
-        <v>58.932155609130859</v>
+        <v>0.73356723785400391</v>
       </c>
       <c r="C8">
-        <v>66.187843322753906</v>
+        <v>0.76083278656005859</v>
       </c>
       <c r="E8">
-        <v>1.3076983690261841</v>
+        <v>1.3170207738876343</v>
       </c>
       <c r="F8">
-        <v>1.2275243997573853</v>
+        <v>1.2886656522750854</v>
       </c>
       <c r="G8">
-        <v>1.3878724575042725</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.3453758955001831</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>65.279998779296875</v>
+        <v>0.77296000719070435</v>
       </c>
       <c r="B9">
-        <v>62.084667205810547</v>
+        <v>0.75990742444992065</v>
       </c>
       <c r="C9">
-        <v>68.475334167480469</v>
+        <v>0.78601258993148804</v>
       </c>
       <c r="E9">
-        <v>1.2485713958740234</v>
+        <v>1.2685384750366211</v>
       </c>
       <c r="F9">
-        <v>1.172243595123291</v>
+        <v>1.243529200553894</v>
       </c>
       <c r="G9">
-        <v>1.3248993158340454</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.2935478687286377</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>67.040000915527344</v>
+        <v>0.78655999898910522</v>
       </c>
       <c r="B10">
-        <v>63.689067840576172</v>
+        <v>0.77362906932830811</v>
       </c>
       <c r="C10">
-        <v>70.39093017578125</v>
+        <v>0.79949092864990234</v>
       </c>
       <c r="E10">
-        <v>1.2146031856536865</v>
+        <v>1.2452138662338257</v>
       </c>
       <c r="F10">
-        <v>1.146522045135498</v>
+        <v>1.2213971614837646</v>
       </c>
       <c r="G10">
-        <v>1.282684326171875</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.2690305709838867</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>65.919998168945313</v>
+        <v>0.80111998319625854</v>
       </c>
       <c r="B11">
-        <v>62.906223297119141</v>
+        <v>0.78844368457794189</v>
       </c>
       <c r="C11">
-        <v>68.93377685546875</v>
+        <v>0.81379634141921997</v>
       </c>
       <c r="E11">
-        <v>1.2314286231994629</v>
+        <v>1.2233299016952515</v>
       </c>
       <c r="F11">
-        <v>1.1692379713058472</v>
+        <v>1.1964647769927979</v>
       </c>
       <c r="G11">
-        <v>1.2936191558837891</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.2501950263977051</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>67.360000610351563</v>
+        <v>0.81455999612808228</v>
       </c>
       <c r="B12">
-        <v>63.879413604736328</v>
+        <v>0.80184060335159302</v>
       </c>
       <c r="C12">
-        <v>70.840583801269531</v>
+        <v>0.82727938890457153</v>
       </c>
       <c r="E12">
-        <v>1.2117459774017334</v>
+        <v>1.2007133960723877</v>
       </c>
       <c r="F12">
-        <v>1.1365017890930176</v>
+        <v>1.1781561374664307</v>
       </c>
       <c r="G12">
-        <v>1.2869902849197388</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.2232707738876343</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>69.599998474121094</v>
+        <v>0.82543998956680298</v>
       </c>
       <c r="B13">
-        <v>66.11016845703125</v>
+        <v>0.81324422359466553</v>
       </c>
       <c r="C13">
-        <v>73.089828491210937</v>
+        <v>0.83763575553894043</v>
       </c>
       <c r="E13">
-        <v>1.1709524393081665</v>
+        <v>1.1821056604385376</v>
       </c>
       <c r="F13">
-        <v>1.1024694442749023</v>
+        <v>1.1616504192352295</v>
       </c>
       <c r="G13">
-        <v>1.2394353151321411</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.2025609016418457</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>69.279998779296875</v>
+        <v>0.83407998085021973</v>
       </c>
       <c r="B14">
-        <v>65.827285766601562</v>
+        <v>0.82244986295700073</v>
       </c>
       <c r="C14">
-        <v>72.732711791992188</v>
+        <v>0.8457101583480835</v>
       </c>
       <c r="E14">
-        <v>1.1759524345397949</v>
+        <v>1.1679757833480835</v>
       </c>
       <c r="F14">
-        <v>1.1080280542373657</v>
+        <v>1.1486247777938843</v>
       </c>
       <c r="G14">
-        <v>1.2438766956329346</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.1873267889022827</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>71.680000305175781</v>
+        <v>0.84112000465393066</v>
       </c>
       <c r="B15">
-        <v>68.706573486328125</v>
+        <v>0.82982927560806274</v>
       </c>
       <c r="C15">
-        <v>74.653427124023438</v>
+        <v>0.85241073369979858</v>
       </c>
       <c r="E15">
-        <v>1.1301587820053101</v>
+        <v>1.1564970016479492</v>
       </c>
       <c r="F15">
-        <v>1.0760053396224976</v>
+        <v>1.1387484073638916</v>
       </c>
       <c r="G15">
-        <v>1.1843122243881226</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.1742455959320068</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>70.080001831054687</v>
+        <v>0.84975999593734741</v>
       </c>
       <c r="B16">
-        <v>66.809944152832031</v>
+        <v>0.83901971578598022</v>
       </c>
       <c r="C16">
-        <v>73.350059509277344</v>
+        <v>0.8605002760887146</v>
       </c>
       <c r="E16">
-        <v>1.1600793600082397</v>
+        <v>1.1430355310440063</v>
       </c>
       <c r="F16">
-        <v>1.0968233346939087</v>
+        <v>1.1264986991882324</v>
       </c>
       <c r="G16">
-        <v>1.2233353853225708</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.1595723628997803</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>71.519996643066406</v>
+        <v>0.85343998670578003</v>
       </c>
       <c r="B17">
-        <v>68.516258239746094</v>
+        <v>0.84287291765213013</v>
       </c>
       <c r="C17">
-        <v>74.52374267578125</v>
+        <v>0.86400711536407471</v>
       </c>
       <c r="E17">
-        <v>1.1329364776611328</v>
+        <v>1.1372554302215576</v>
       </c>
       <c r="F17">
-        <v>1.0783891677856445</v>
+        <v>1.1216062307357788</v>
       </c>
       <c r="G17">
-        <v>1.1874839067459106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.1529045104980469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>72.319999694824219</v>
+        <v>0.85887998342514038</v>
       </c>
       <c r="B18">
-        <v>69.55712890625</v>
+        <v>0.8479427695274353</v>
       </c>
       <c r="C18">
-        <v>75.082870483398438</v>
+        <v>0.86981719732284546</v>
       </c>
       <c r="E18">
-        <v>1.1173809766769409</v>
+        <v>1.1309342384338379</v>
       </c>
       <c r="F18">
-        <v>1.0710018873214722</v>
+        <v>1.1147351264953613</v>
       </c>
       <c r="G18">
-        <v>1.1637599468231201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.1471333503723145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>71.680000305175781</v>
+        <v>0.86176002025604248</v>
       </c>
       <c r="B19">
-        <v>68.845207214355469</v>
+        <v>0.85158246755599976</v>
       </c>
       <c r="C19">
-        <v>74.514793395996094</v>
+        <v>0.87193757295608521</v>
       </c>
       <c r="E19">
-        <v>1.1288095712661743</v>
+        <v>1.1252796649932861</v>
       </c>
       <c r="F19">
-        <v>1.0773776769638062</v>
+        <v>1.1103427410125732</v>
       </c>
       <c r="G19">
-        <v>1.1802414655685425</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.140216588973999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>71.680000305175781</v>
+        <v>0.86303997039794922</v>
       </c>
       <c r="B20">
-        <v>69.066909790039062</v>
+        <v>0.85273200273513794</v>
       </c>
       <c r="C20">
-        <v>74.2930908203125</v>
+        <v>0.87334799766540527</v>
       </c>
       <c r="E20">
-        <v>1.126031756401062</v>
+        <v>1.1241039037704468</v>
       </c>
       <c r="F20">
-        <v>1.0827798843383789</v>
+        <v>1.1086244583129883</v>
       </c>
       <c r="G20">
-        <v>1.1692835092544556</v>
+        <v>1.1395833492279053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data is good to go!
</commit_message>
<xml_diff>
--- a/Assn1/OutputData/test_blockSizeGreaterThanOne.xlsx
+++ b/Assn1/OutputData/test_blockSizeGreaterThanOne.xlsx
@@ -24,7 +24,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>BlockCount</t>
+  </si>
   <si>
     <t>Throughput</t>
   </si>
@@ -359,410 +362,332 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>0.39392000436782837</v>
       </c>
-      <c r="B2">
+      <c r="D2">
         <v>0.37689036130905151</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>0.41094964742660522</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>2.8668475151062012</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>2.6732652187347412</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>3.0604300498962402</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>0.52351999282836914</v>
-      </c>
-      <c r="B3">
-        <v>0.50625449419021606</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0.54078549146652222</v>
+        <v>0.48032000660896301</v>
+      </c>
+      <c r="D3">
+        <v>0.46388769149780273</v>
       </c>
       <c r="E3">
-        <v>2.0024442672729492</v>
-      </c>
-      <c r="F3">
-        <v>1.9128973484039307</v>
+        <v>0.4967522919178009</v>
       </c>
       <c r="G3">
-        <v>2.0919909477233887</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2.0196619033813477</v>
+      </c>
+      <c r="H3">
+        <v>1.918787956237793</v>
+      </c>
+      <c r="I3">
+        <v>2.1205358505249023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>0.60048002004623413</v>
-      </c>
-      <c r="B4">
-        <v>0.58450525999069214</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>0.61645478010177612</v>
+        <v>0.5987200140953064</v>
+      </c>
+      <c r="D4">
+        <v>0.58368951082229614</v>
       </c>
       <c r="E4">
-        <v>1.6865731477737427</v>
-      </c>
-      <c r="F4">
-        <v>1.6304736137390137</v>
+        <v>0.61375045776367188</v>
       </c>
       <c r="G4">
-        <v>1.7426726818084717</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.547599196434021</v>
+      </c>
+      <c r="H4">
+        <v>1.4949449300765991</v>
+      </c>
+      <c r="I4">
+        <v>1.6002535820007324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>0.65087997913360596</v>
-      </c>
-      <c r="B5">
-        <v>0.63519388437271118</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>0.66656613349914551</v>
+        <v>0.63871997594833374</v>
+      </c>
+      <c r="D5">
+        <v>0.62428659200668335</v>
       </c>
       <c r="E5">
-        <v>1.5434224605560303</v>
-      </c>
-      <c r="F5">
-        <v>1.4946485757827759</v>
+        <v>0.65315335988998413</v>
       </c>
       <c r="G5">
-        <v>1.5921964645385742</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.4423190355300903</v>
+      </c>
+      <c r="H5">
+        <v>1.3914345502853394</v>
+      </c>
+      <c r="I5">
+        <v>1.4932035207748413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>0.69488000869750977</v>
-      </c>
-      <c r="B6">
-        <v>0.67959630489349365</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>0.71016371250152588</v>
+        <v>0.71087998151779175</v>
+      </c>
+      <c r="D6">
+        <v>0.69852268695831299</v>
       </c>
       <c r="E6">
-        <v>1.4430468082427979</v>
-      </c>
-      <c r="F6">
-        <v>1.391973614692688</v>
+        <v>0.72323733568191528</v>
       </c>
       <c r="G6">
-        <v>1.4941198825836182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.2661213874816895</v>
+      </c>
+      <c r="H6">
+        <v>1.2402869462966919</v>
+      </c>
+      <c r="I6">
+        <v>1.2919559478759766</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>0.72703999280929565</v>
-      </c>
-      <c r="B7">
-        <v>0.71297943592071533</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>0.74110054969787598</v>
+        <v>0.73280000686645508</v>
+      </c>
+      <c r="D7">
+        <v>0.72074472904205322</v>
       </c>
       <c r="E7">
-        <v>1.361954927444458</v>
-      </c>
-      <c r="F7">
-        <v>1.3231201171875</v>
+        <v>0.74485528469085693</v>
       </c>
       <c r="G7">
-        <v>1.400789737701416</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.2279452085494995</v>
+      </c>
+      <c r="H7">
+        <v>1.2003469467163086</v>
+      </c>
+      <c r="I7">
+        <v>1.25554358959198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>0.74720001220703125</v>
-      </c>
-      <c r="B8">
-        <v>0.73356723785400391</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>0.76083278656005859</v>
+        <v>0.78175997734069824</v>
+      </c>
+      <c r="D8">
+        <v>0.77181828022003174</v>
       </c>
       <c r="E8">
-        <v>1.3170207738876343</v>
-      </c>
-      <c r="F8">
-        <v>1.2886656522750854</v>
+        <v>0.79170173406600952</v>
       </c>
       <c r="G8">
-        <v>1.3453758955001831</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.1387587785720825</v>
+      </c>
+      <c r="H8">
+        <v>1.1226532459259033</v>
+      </c>
+      <c r="I8">
+        <v>1.1548641920089722</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>0.77296000719070435</v>
-      </c>
-      <c r="B9">
-        <v>0.75990742444992065</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>0.78601258993148804</v>
+        <v>0.79824000597000122</v>
+      </c>
+      <c r="D9">
+        <v>0.7888215184211731</v>
       </c>
       <c r="E9">
-        <v>1.2685384750366211</v>
-      </c>
-      <c r="F9">
-        <v>1.243529200553894</v>
+        <v>0.80765849351882935</v>
       </c>
       <c r="G9">
-        <v>1.2935478687286377</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.1138293743133545</v>
+      </c>
+      <c r="H9">
+        <v>1.0985566377639771</v>
+      </c>
+      <c r="I9">
+        <v>1.1291021108627319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>0.78655999898910522</v>
-      </c>
-      <c r="B10">
-        <v>0.77362906932830811</v>
+        <v>25</v>
       </c>
       <c r="C10">
-        <v>0.79949092864990234</v>
+        <v>0.81519997119903564</v>
+      </c>
+      <c r="D10">
+        <v>0.80663686990737915</v>
       </c>
       <c r="E10">
-        <v>1.2452138662338257</v>
-      </c>
-      <c r="F10">
-        <v>1.2213971614837646</v>
+        <v>0.82376313209533691</v>
       </c>
       <c r="G10">
-        <v>1.2690305709838867</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.0879595279693604</v>
+      </c>
+      <c r="H10">
+        <v>1.0754296779632568</v>
+      </c>
+      <c r="I10">
+        <v>1.1004893779754639</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>0.80111998319625854</v>
-      </c>
-      <c r="B11">
-        <v>0.78844368457794189</v>
+        <v>32</v>
       </c>
       <c r="C11">
-        <v>0.81379634141921997</v>
+        <v>0.82687997817993164</v>
+      </c>
+      <c r="D11">
+        <v>0.81934070587158203</v>
       </c>
       <c r="E11">
-        <v>1.2233299016952515</v>
-      </c>
-      <c r="F11">
-        <v>1.1964647769927979</v>
+        <v>0.83441931009292603</v>
       </c>
       <c r="G11">
-        <v>1.2501950263977051</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.0705373287200928</v>
+      </c>
+      <c r="H11">
+        <v>1.0598032474517822</v>
+      </c>
+      <c r="I11">
+        <v>1.0812714099884033</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>0.81455999612808228</v>
-      </c>
-      <c r="B12">
-        <v>0.80184060335159302</v>
+        <v>40</v>
       </c>
       <c r="C12">
-        <v>0.82727938890457153</v>
+        <v>0.83568000793457031</v>
+      </c>
+      <c r="D12">
+        <v>0.82874155044555664</v>
       </c>
       <c r="E12">
-        <v>1.2007133960723877</v>
-      </c>
-      <c r="F12">
-        <v>1.1781561374664307</v>
+        <v>0.84261840581893921</v>
       </c>
       <c r="G12">
-        <v>1.2232707738876343</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.058150053024292</v>
+      </c>
+      <c r="H12">
+        <v>1.0485970973968506</v>
+      </c>
+      <c r="I12">
+        <v>1.0677028894424438</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>0.82543998956680298</v>
-      </c>
-      <c r="B13">
-        <v>0.81324422359466553</v>
+        <v>50</v>
       </c>
       <c r="C13">
-        <v>0.83763575553894043</v>
+        <v>0.84656000137329102</v>
+      </c>
+      <c r="D13">
+        <v>0.84046977758407593</v>
       </c>
       <c r="E13">
-        <v>1.1821056604385376</v>
-      </c>
-      <c r="F13">
-        <v>1.1616504192352295</v>
+        <v>0.8526502251625061</v>
       </c>
       <c r="G13">
-        <v>1.2025609016418457</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.0432833433151245</v>
+      </c>
+      <c r="H13">
+        <v>1.0351431369781494</v>
+      </c>
+      <c r="I13">
+        <v>1.0514235496520996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>0.83407998085021973</v>
-      </c>
-      <c r="B14">
-        <v>0.82244986295700073</v>
+        <v>80</v>
       </c>
       <c r="C14">
-        <v>0.8457101583480835</v>
+        <v>0.78127998113632202</v>
+      </c>
+      <c r="D14">
+        <v>0.77658271789550781</v>
       </c>
       <c r="E14">
-        <v>1.1679757833480835</v>
-      </c>
-      <c r="F14">
-        <v>1.1486247777938843</v>
+        <v>0.78597730398178101</v>
       </c>
       <c r="G14">
-        <v>1.1873267889022827</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>0.84112000465393066</v>
-      </c>
-      <c r="B15">
-        <v>0.82982927560806274</v>
-      </c>
-      <c r="C15">
-        <v>0.85241073369979858</v>
-      </c>
-      <c r="E15">
-        <v>1.1564970016479492</v>
-      </c>
-      <c r="F15">
-        <v>1.1387484073638916</v>
-      </c>
-      <c r="G15">
-        <v>1.1742455959320068</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>0.84975999593734741</v>
-      </c>
-      <c r="B16">
-        <v>0.83901971578598022</v>
-      </c>
-      <c r="C16">
-        <v>0.8605002760887146</v>
-      </c>
-      <c r="E16">
-        <v>1.1430355310440063</v>
-      </c>
-      <c r="F16">
-        <v>1.1264986991882324</v>
-      </c>
-      <c r="G16">
-        <v>1.1595723628997803</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>0.85343998670578003</v>
-      </c>
-      <c r="B17">
-        <v>0.84287291765213013</v>
-      </c>
-      <c r="C17">
-        <v>0.86400711536407471</v>
-      </c>
-      <c r="E17">
-        <v>1.1372554302215576</v>
-      </c>
-      <c r="F17">
-        <v>1.1216062307357788</v>
-      </c>
-      <c r="G17">
-        <v>1.1529045104980469</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>0.85887998342514038</v>
-      </c>
-      <c r="B18">
-        <v>0.8479427695274353</v>
-      </c>
-      <c r="C18">
-        <v>0.86981719732284546</v>
-      </c>
-      <c r="E18">
-        <v>1.1309342384338379</v>
-      </c>
-      <c r="F18">
-        <v>1.1147351264953613</v>
-      </c>
-      <c r="G18">
-        <v>1.1471333503723145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>0.86176002025604248</v>
-      </c>
-      <c r="B19">
-        <v>0.85158246755599976</v>
-      </c>
-      <c r="C19">
-        <v>0.87193757295608521</v>
-      </c>
-      <c r="E19">
-        <v>1.1252796649932861</v>
-      </c>
-      <c r="F19">
-        <v>1.1103427410125732</v>
-      </c>
-      <c r="G19">
-        <v>1.140216588973999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>0.86303997039794922</v>
-      </c>
-      <c r="B20">
-        <v>0.85273200273513794</v>
-      </c>
-      <c r="C20">
-        <v>0.87334799766540527</v>
-      </c>
-      <c r="E20">
-        <v>1.1241039037704468</v>
-      </c>
-      <c r="F20">
-        <v>1.1086244583129883</v>
-      </c>
-      <c r="G20">
-        <v>1.1395833492279053</v>
+        <v>1.0266110897064209</v>
+      </c>
+      <c r="H14">
+        <v>1.0197902917861938</v>
+      </c>
+      <c r="I14">
+        <v>1.0334318876266479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed up formatting, added throughput vs block size
</commit_message>
<xml_diff>
--- a/Assn1/OutputData/test_blockSizeGreaterThanOne.xlsx
+++ b/Assn1/OutputData/test_blockSizeGreaterThanOne.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16180" windowHeight="9500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16180" windowHeight="7150"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -362,7 +362,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -690,6 +690,144 @@
         <v>1.0334318876266479</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>0.78575998544692993</v>
+      </c>
+      <c r="D15">
+        <v>0.78165715932846069</v>
+      </c>
+      <c r="E15">
+        <v>0.78986287117004395</v>
+      </c>
+      <c r="G15">
+        <v>1.020111083984375</v>
+      </c>
+      <c r="H15">
+        <v>1.0142205953598022</v>
+      </c>
+      <c r="I15">
+        <v>1.0260015726089478</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>125</v>
+      </c>
+      <c r="C16">
+        <v>0.78816002607345581</v>
+      </c>
+      <c r="D16">
+        <v>0.78446555137634277</v>
+      </c>
+      <c r="E16">
+        <v>0.79185444116592407</v>
+      </c>
+      <c r="G16">
+        <v>1.0166110992431641</v>
+      </c>
+      <c r="H16">
+        <v>1.0113708972930908</v>
+      </c>
+      <c r="I16">
+        <v>1.0218513011932373</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>160</v>
+      </c>
+      <c r="C17">
+        <v>0.79119998216629028</v>
+      </c>
+      <c r="D17">
+        <v>0.78784477710723877</v>
+      </c>
+      <c r="E17">
+        <v>0.79455524682998657</v>
+      </c>
+      <c r="G17">
+        <v>1.0124444961547852</v>
+      </c>
+      <c r="H17">
+        <v>1.0076224803924561</v>
+      </c>
+      <c r="I17">
+        <v>1.0172665119171143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>200</v>
+      </c>
+      <c r="C18">
+        <v>0.79280000925064087</v>
+      </c>
+      <c r="D18">
+        <v>0.78968936204910278</v>
+      </c>
+      <c r="E18">
+        <v>0.79591065645217896</v>
+      </c>
+      <c r="G18">
+        <v>1.0102221965789795</v>
+      </c>
+      <c r="H18">
+        <v>1.0057259798049927</v>
+      </c>
+      <c r="I18">
+        <v>1.0147185325622559</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>250</v>
+      </c>
+      <c r="C19">
+        <v>0.71487998962402344</v>
+      </c>
+      <c r="D19">
+        <v>0.71236681938171387</v>
+      </c>
+      <c r="E19">
+        <v>0.71739315986633301</v>
+      </c>
+      <c r="G19">
+        <v>1.0080714225769043</v>
+      </c>
+      <c r="H19">
+        <v>1.0040723085403442</v>
+      </c>
+      <c r="I19">
+        <v>1.0120705366134644</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>400</v>
+      </c>
+      <c r="C20">
+        <v>0.71711999177932739</v>
+      </c>
+      <c r="D20">
+        <v>0.71526795625686646</v>
+      </c>
+      <c r="E20">
+        <v>0.71897202730178833</v>
+      </c>
+      <c r="G20">
+        <v>1.0045000314712524</v>
+      </c>
+      <c r="H20">
+        <v>1.0016062259674072</v>
+      </c>
+      <c r="I20">
+        <v>1.0073938369750977</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>